<commit_message>
mantenimiento inspeccion y parte de inventario
</commit_message>
<xml_diff>
--- a/Informacion plantillas/01- Informacion de Perfiles y Colaboradores VD 01.xlsx
+++ b/Informacion plantillas/01- Informacion de Perfiles y Colaboradores VD 01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\06-MANTENIMIENTO\Formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\06-MANTENIMIENTO\Formatos\Elkin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB38E85-1F8F-4AE1-8B98-125B0A082495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4587F66-B5C1-43A1-9F0B-2F95A8FE34F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="858" xr2:uid="{4FDF128A-31F3-49CB-93DC-0573771C02A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="858" firstSheet="1" activeTab="9" xr2:uid="{4FDF128A-31F3-49CB-93DC-0573771C02A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Perfiles de Acceso" sheetId="10" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="39">
   <si>
     <t xml:space="preserve">DATOS DEL TRABAJADOR </t>
   </si>
@@ -250,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,6 +258,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,21 +290,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,6 +382,104 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>784861</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>563881</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>92605</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46048123-C64A-5D00-540B-DCADA99C88FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="784861" y="68581"/>
+          <a:ext cx="1249680" cy="1487064"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7621</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>15241</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DAF54FF-7585-AE15-06E1-BC02472702C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800101" y="22860"/>
+          <a:ext cx="1264920" cy="1607820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -446,20 +542,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>413282</xdr:colOff>
+      <xdr:colOff>411480</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>181030</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -489,8 +585,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="960120" y="22860"/>
-          <a:ext cx="1038122" cy="1577340"/>
+          <a:off x="883920" y="0"/>
+          <a:ext cx="1112520" cy="1644070"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -512,7 +608,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -578,7 +674,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -644,20 +740,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>579647</xdr:colOff>
+      <xdr:colOff>602507</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -687,7 +783,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="906780" y="83820"/>
+          <a:off x="929640" y="114300"/>
           <a:ext cx="1257827" cy="1516380"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -710,7 +806,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1058,32 +1154,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D804763-1F82-48FB-A45C-3EA16AC02888}">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1092,10 +1188,10 @@
       <c r="D5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1229,107 +1325,118 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F9A412-9229-41CB-9343-BEF6FDB4940A}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>80110706</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B1:C9"/>
+    <mergeCell ref="A1:A9"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B1:C9"/>
-    <mergeCell ref="A1:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1351,99 +1458,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>1019099601</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1465,7 +1572,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1475,111 +1582,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>1045235120</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:A9"/>
+    <mergeCell ref="B1:C9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A1:A9"/>
-    <mergeCell ref="B1:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1588,7 +1696,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1598,111 +1706,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>8604171</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:C9"/>
+    <mergeCell ref="A1:A9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B1:C9"/>
-    <mergeCell ref="A1:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1721,109 +1830,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>1063277243</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:C9"/>
+    <mergeCell ref="A1:A9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B1:C9"/>
-    <mergeCell ref="A1:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1835,7 +1944,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1844,109 +1953,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>3738908</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:C9"/>
+    <mergeCell ref="A1:A9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B1:C9"/>
-    <mergeCell ref="A1:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1958,115 +2067,115 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>1047438805</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:C9"/>
+    <mergeCell ref="A1:A9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B1:C9"/>
-    <mergeCell ref="A1:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2087,109 +2196,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>1019099601</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:C9"/>
+    <mergeCell ref="A1:A9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B1:C9"/>
-    <mergeCell ref="A1:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2201,7 +2310,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2210,109 +2319,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>5820371</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:C9"/>
+    <mergeCell ref="A1:A9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B1:C9"/>
-    <mergeCell ref="A1:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>